<commit_message>
special drop down method add
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/PropertyCreate.xlsx
+++ b/src/main/resources/dataCreate/PropertyCreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\seleniumAmtTesting\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C7177-C27D-4E78-8247-002CDCF5A0ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD001B72-CFCC-45F7-A351-57F46C6D2693}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="194">
   <si>
     <t>TC_ID</t>
   </si>
@@ -611,10 +611,7 @@
     <t>autoManage</t>
   </si>
   <si>
-    <t>test_test_252</t>
-  </si>
-  <si>
-    <t>test_test_254</t>
+    <t>test_test_257</t>
   </si>
 </sst>
 </file>
@@ -44902,7 +44899,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44984,10 +44981,10 @@
         <v>168</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D2" s="80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="80" t="s">
         <v>167</v>
@@ -45030,54 +45027,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="80" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>193</v>
-      </c>
-      <c r="E3" s="80" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="80" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3">
-        <v>1229</v>
-      </c>
-      <c r="I3" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="J3" s="80" t="s">
-        <v>172</v>
-      </c>
-      <c r="K3" s="80" t="s">
-        <v>173</v>
-      </c>
-      <c r="L3" s="80" t="s">
-        <v>174</v>
-      </c>
-      <c r="M3">
-        <v>12</v>
-      </c>
-      <c r="N3" s="80" t="s">
-        <v>175</v>
-      </c>
-      <c r="O3" s="80" t="s">
-        <v>176</v>
-      </c>
-      <c r="P3" s="80" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>1</v>
-      </c>
+      <c r="A3" s="79"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add property and lease
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/PropertyCreate.xlsx
+++ b/src/main/resources/dataCreate/PropertyCreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\FinalTestAMT\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\seleniumAmtTesting\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C28290-526C-4839-A50C-36C707A8147E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3226D7AD-F989-43A7-A178-0805AA54A658}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="330" windowWidth="19440" windowHeight="15150" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="209">
   <si>
     <t>TC_ID</t>
   </si>
@@ -612,9 +612,6 @@
     <t>autoManage</t>
   </si>
   <si>
-    <t>test_test_257</t>
-  </si>
-  <si>
     <t>TestId</t>
   </si>
   <si>
@@ -639,12 +636,6 @@
     <t>expirationDate</t>
   </si>
   <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>1.Sumaiya property</t>
-  </si>
-  <si>
     <t>Test_L</t>
   </si>
   <si>
@@ -662,6 +653,12 @@
   <si>
     <t>01</t>
   </si>
+  <si>
+    <t>contractTerm</t>
+  </si>
+  <si>
+    <t>test_test_368</t>
+  </si>
 </sst>
 </file>
 
@@ -670,11 +667,18 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -949,26 +953,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -989,7 +993,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1069,7 +1073,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1132,7 +1136,7 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1144,7 +1148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1166,36 +1170,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1207,7 +1211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -44712,7 +44722,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="29" operator="equal" id="{BC2517B2-EF00-4DD7-BFDB-45CBEA86F95A}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44725,7 +44735,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="27" operator="equal" id="{189AF047-2FB8-4A30-9CF7-715E6643A0DD}">
-            <xm:f>'\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44735,7 +44745,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="28" operator="equal" id="{6D03C738-803D-4D93-96DB-E16020106ABC}">
-            <xm:f>'\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44748,7 +44758,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="26" operator="equal" id="{56C5208A-0418-4DF5-B7BC-BF1068251FBD}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44761,7 +44771,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="25" operator="equal" id="{F9A80D82-E708-49D9-8A9A-03A9E48C75D6}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44774,7 +44784,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="22" operator="equal" id="{0D5C99F4-1393-4655-A002-2C74CAC6E98D}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44784,7 +44794,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="23" operator="equal" id="{D3BAE2B6-788D-4F7E-9F77-64B679D84250}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44797,7 +44807,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="21" operator="equal" id="{19F09A0D-E228-4618-996A-D73A57873828}">
-            <xm:f>'\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44810,7 +44820,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="19" operator="equal" id="{A5EB4A4C-92D1-401A-A8A6-95F55ADA941C}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44823,7 +44833,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="18" operator="equal" id="{EB04725F-DD9A-4E48-B06D-A19DB4615166}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44836,7 +44846,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="15" operator="equal" id="{2EEC973A-04A6-4813-8C3F-A9DF77292B01}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44846,7 +44856,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="16" operator="equal" id="{4133868E-335E-4598-A3E1-F0F9ECCCAB39}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44859,7 +44869,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="14" operator="equal" id="{6FC88015-4D02-4917-844B-7BD94C0F201B}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44872,7 +44882,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="11" operator="equal" id="{526BD5E8-3A68-4932-9848-428C4F00E27C}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44882,7 +44892,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="12" operator="equal" id="{7900C41F-32F5-414D-B3F9-11BD7A0F0312}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44895,7 +44905,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="10" operator="equal" id="{01594AD9-16DD-4CBF-801D-EEB0EF3BAC6A}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44908,7 +44918,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="8" operator="equal" id="{DCD056FF-A462-4A08-BE97-F988112DD0C6}">
-            <xm:f>'\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44921,7 +44931,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="7" operator="equal" id="{38A3F3E9-5AF4-4B13-96A1-65DE688F4CFB}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44934,7 +44944,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="4" operator="equal" id="{8C16CCA5-35EE-4D6B-B4ED-61524C363BE1}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44944,7 +44954,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="5" operator="equal" id="{90BAD57D-85B5-4545-BD61-3031E0C1837F}">
-            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44957,7 +44967,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="3" operator="equal" id="{1BDB983F-3025-482D-BCAF-4327ACC215C8}">
-            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44970,7 +44980,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="1" operator="equal" id="{60F9AD86-5185-4E91-BD53-04AF4E3F10F8}">
-            <xm:f>'\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'C:\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -45007,8 +45017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81362EF-F639-4F16-9B39-A84C1506E605}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45090,10 +45100,10 @@
         <v>168</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="D2" s="80" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="E2" s="80" t="s">
         <v>167</v>
@@ -45158,10 +45168,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEB6E0A-2F06-410F-BCB9-2F2C2849D4D7}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45175,11 +45185,12 @@
     <col min="7" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B1" s="82" t="s">
         <v>166</v>
@@ -45188,28 +45199,28 @@
         <v>178</v>
       </c>
       <c r="D1" s="83" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="83" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="F1" s="83" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="G1" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="H1" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="H1" s="85" t="s">
+      <c r="I1" s="83" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="J1" s="86" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="86" t="s">
-        <v>201</v>
-      </c>
-      <c r="K1" s="81" t="s">
-        <v>202</v>
+      <c r="K1" s="90" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -45218,10 +45229,10 @@
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="89" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D2" s="88" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E2" s="88">
         <v>1234</v>
@@ -45230,25 +45241,29 @@
         <v>173</v>
       </c>
       <c r="G2" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="88" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="87" t="s">
+        <v>204</v>
+      </c>
+      <c r="J2" s="87" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="88" t="s">
+      <c r="K2" s="91" t="s">
         <v>206</v>
       </c>
-      <c r="I2" s="87" t="s">
-        <v>207</v>
-      </c>
-      <c r="J2" s="87" t="s">
-        <v>208</v>
-      </c>
-      <c r="K2" s="87" t="s">
-        <v>209</v>
-      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="89"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: This will create lease
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/PropertyCreate.xlsx
+++ b/src/main/resources/dataCreate/PropertyCreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\seleniumAmtTesting\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTTestingFramework\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3226D7AD-F989-43A7-A178-0805AA54A658}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6F6D57-D89A-462C-A13B-16F3A8032217}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="210">
   <si>
     <t>TC_ID</t>
   </si>
@@ -636,16 +636,10 @@
     <t>expirationDate</t>
   </si>
   <si>
-    <t>Test_L</t>
-  </si>
-  <si>
     <t>Base Year</t>
   </si>
   <si>
     <t>Income</t>
-  </si>
-  <si>
-    <t>11/01/2017</t>
   </si>
   <si>
     <t>12/31/2026</t>
@@ -657,7 +651,16 @@
     <t>contractTerm</t>
   </si>
   <si>
-    <t>test_test_368</t>
+    <t>01/01/2017</t>
+  </si>
+  <si>
+    <t>P_Test_Property</t>
+  </si>
+  <si>
+    <t>Test_00001_lease_01</t>
+  </si>
+  <si>
+    <t>00001.01</t>
   </si>
 </sst>
 </file>
@@ -955,7 +958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1217,6 +1220,9 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -44722,7 +44728,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="29" operator="equal" id="{BC2517B2-EF00-4DD7-BFDB-45CBEA86F95A}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44735,7 +44741,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="27" operator="equal" id="{189AF047-2FB8-4A30-9CF7-715E6643A0DD}">
-            <xm:f>'C:\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44745,7 +44751,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="28" operator="equal" id="{6D03C738-803D-4D93-96DB-E16020106ABC}">
-            <xm:f>'C:\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\10-12-nous\AMTDirect_NousAutomation\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44758,7 +44764,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="26" operator="equal" id="{56C5208A-0418-4DF5-B7BC-BF1068251FBD}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44771,7 +44777,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="25" operator="equal" id="{F9A80D82-E708-49D9-8A9A-03A9E48C75D6}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44784,7 +44790,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="22" operator="equal" id="{0D5C99F4-1393-4655-A002-2C74CAC6E98D}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44794,7 +44800,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="23" operator="equal" id="{D3BAE2B6-788D-4F7E-9F77-64B679D84250}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44807,7 +44813,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="21" operator="equal" id="{19F09A0D-E228-4618-996A-D73A57873828}">
-            <xm:f>'C:\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44820,7 +44826,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="19" operator="equal" id="{A5EB4A4C-92D1-401A-A8A6-95F55ADA941C}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44833,7 +44839,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="18" operator="equal" id="{EB04725F-DD9A-4E48-B06D-A19DB4615166}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44846,7 +44852,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="15" operator="equal" id="{2EEC973A-04A6-4813-8C3F-A9DF77292B01}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44856,7 +44862,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="16" operator="equal" id="{4133868E-335E-4598-A3E1-F0F9ECCCAB39}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44869,7 +44875,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="14" operator="equal" id="{6FC88015-4D02-4917-844B-7BD94C0F201B}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44882,7 +44888,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="11" operator="equal" id="{526BD5E8-3A68-4932-9848-428C4F00E27C}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44892,7 +44898,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="12" operator="equal" id="{7900C41F-32F5-414D-B3F9-11BD7A0F0312}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44905,7 +44911,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="10" operator="equal" id="{01594AD9-16DD-4CBF-801D-EEB0EF3BAC6A}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44918,7 +44924,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="8" operator="equal" id="{DCD056FF-A462-4A08-BE97-F988112DD0C6}">
-            <xm:f>'C:\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44931,7 +44937,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="7" operator="equal" id="{38A3F3E9-5AF4-4B13-96A1-65DE688F4CFB}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44944,7 +44950,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="4" operator="equal" id="{8C16CCA5-35EE-4D6B-B4ED-61524C363BE1}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44954,7 +44960,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="5" operator="equal" id="{90BAD57D-85B5-4545-BD61-3031E0C1837F}">
-            <xm:f>'C:\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\AMT Project Suite\22-10-2018\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44967,7 +44973,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="3" operator="equal" id="{1BDB983F-3025-482D-BCAF-4327ACC215C8}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -44980,7 +44986,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="1" operator="equal" id="{60F9AD86-5185-4E91-BD53-04AF4E3F10F8}">
-            <xm:f>'C:\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
+            <xm:f>'\temp\seleniumAmtTesting\Framework\Modules\[FASB.xlsx]Controller'!#REF!</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -45017,8 +45023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81362EF-F639-4F16-9B39-A84C1506E605}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45100,10 +45106,10 @@
         <v>168</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="80" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="D2" s="80">
+        <v>24343465</v>
       </c>
       <c r="E2" s="80" t="s">
         <v>167</v>
@@ -45170,17 +45176,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEB6E0A-2F06-410F-BCB9-2F2C2849D4D7}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="73" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="5" max="5" width="20" style="73" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="7" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
@@ -45201,7 +45207,7 @@
       <c r="D1" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="92" t="s">
         <v>195</v>
       </c>
       <c r="F1" s="83" t="s">
@@ -45220,7 +45226,7 @@
         <v>200</v>
       </c>
       <c r="K1" s="90" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -45228,36 +45234,44 @@
         <v>168</v>
       </c>
       <c r="B2" s="88"/>
-      <c r="C2" s="89" t="s">
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="89" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="88" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" s="88">
-        <v>1234</v>
+      <c r="E2" s="91" t="s">
+        <v>209</v>
       </c>
       <c r="F2" s="88" t="s">
         <v>173</v>
       </c>
       <c r="G2" s="88" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="88" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="88" t="s">
+      <c r="I2" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" s="87" t="s">
         <v>203</v>
       </c>
-      <c r="I2" s="87" t="s">
+      <c r="K2" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="J2" s="87" t="s">
-        <v>205</v>
-      </c>
-      <c r="K2" s="91" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="89"/>
+      <c r="A3" s="79"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="91"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1">

</xml_diff>

<commit_message>
Add: Search a lease
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/PropertyCreate.xlsx
+++ b/src/main/resources/dataCreate/PropertyCreate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTTestingFramework\seleniumTestingFramework\src\main\resources\dataCreate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTAutomatedTesting\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6F6D57-D89A-462C-A13B-16F3A8032217}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEAA02B-4163-49FD-85ED-FF10B52167E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,21 @@
     <sheet name="TC001_TC050" sheetId="3" r:id="rId3"/>
     <sheet name="Property" sheetId="4" r:id="rId4"/>
     <sheet name="Lease" sheetId="5" r:id="rId5"/>
+    <sheet name="Space" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="215">
   <si>
     <t>TC_ID</t>
   </si>
@@ -661,6 +662,21 @@
   </si>
   <si>
     <t>00001.01</t>
+  </si>
+  <si>
+    <t>LeaseName</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Test_00001_lease_04</t>
+  </si>
+  <si>
+    <t>Test_004</t>
   </si>
 </sst>
 </file>
@@ -45176,8 +45192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEB6E0A-2F06-410F-BCB9-2F2C2849D4D7}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45280,4 +45296,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD612C6E-0C35-4A08-BC9E-BAB6CEE21F73}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
work partial for space create
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/PropertyCreate.xlsx
+++ b/src/main/resources/dataCreate/PropertyCreate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTAutomatedTesting\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEAA02B-4163-49FD-85ED-FF10B52167E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C91889-5B4B-4724-8A14-5FFDDD98DC41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -658,12 +658,6 @@
     <t>P_Test_Property</t>
   </si>
   <si>
-    <t>Test_00001_lease_01</t>
-  </si>
-  <si>
-    <t>00001.01</t>
-  </si>
-  <si>
     <t>LeaseName</t>
   </si>
   <si>
@@ -676,7 +670,13 @@
     <t>Test_00001_lease_04</t>
   </si>
   <si>
-    <t>Test_004</t>
+    <t>Test_04</t>
+  </si>
+  <si>
+    <t>Test_00002_lease_09</t>
+  </si>
+  <si>
+    <t>00002.09</t>
   </si>
 </sst>
 </file>
@@ -45192,8 +45192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEB6E0A-2F06-410F-BCB9-2F2C2849D4D7}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45254,10 +45254,10 @@
         <v>207</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F2" s="88" t="s">
         <v>173</v>
@@ -45302,8 +45302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD612C6E-0C35-4A08-BC9E-BAB6CEE21F73}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45319,13 +45319,13 @@
         <v>193</v>
       </c>
       <c r="B1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" t="s">
         <v>210</v>
-      </c>
-      <c r="C1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -45333,10 +45333,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D2">
         <v>1</v>

</xml_diff>

<commit_message>
Add: UICheckbox,Create multi Lease and Update: Clean code
</commit_message>
<xml_diff>
--- a/src/main/resources/dataCreate/PropertyCreate.xlsx
+++ b/src/main/resources/dataCreate/PropertyCreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTAutomatedTesting\seleniumTestingFramework\src\main\resources\dataCreate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C91889-5B4B-4724-8A14-5FFDDD98DC41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985949AE-8EDF-4F08-89A8-6B4A1CDFE1C7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="218">
   <si>
     <t>TC_ID</t>
   </si>
@@ -667,16 +667,25 @@
     <t>Floor</t>
   </si>
   <si>
-    <t>Test_00001_lease_04</t>
+    <t>Test_00002_lease_16</t>
   </si>
   <si>
-    <t>Test_04</t>
+    <t>Test_019</t>
   </si>
   <si>
-    <t>Test_00002_lease_09</t>
+    <t>Test_020</t>
   </si>
   <si>
-    <t>00002.09</t>
+    <t>Test_00002_lease_19</t>
+  </si>
+  <si>
+    <t>Test_00002_lease_20</t>
+  </si>
+  <si>
+    <t>00002.19</t>
+  </si>
+  <si>
+    <t>00002.20</t>
   </si>
 </sst>
 </file>
@@ -45193,7 +45202,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45254,10 +45263,10 @@
         <v>207</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F2" s="88" t="s">
         <v>173</v>
@@ -45279,15 +45288,37 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="91"/>
+      <c r="A3" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="88"/>
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>201</v>
+      </c>
+      <c r="H3" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3" s="87" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="91" t="s">
+        <v>204</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1">
@@ -45300,10 +45331,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD612C6E-0C35-4A08-BC9E-BAB6CEE21F73}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45342,6 +45373,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>